<commit_message>
updated and added example files in larray/tests/data + added get_example_filepath() function
</commit_message>
<xml_diff>
--- a/larray/tests/data/examples.xlsx
+++ b/larray/tests/data/examples.xlsx
@@ -1,73 +1,67 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ald\Projects\larray\larray\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F7045E0-7DB7-412E-8D92-B06D3D9338B6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083B36A3-412C-4F86-872C-2976BE7F79A2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="12705" activeTab="3" xr2:uid="{7043041A-E710-461B-9144-9DDB3B96D9FD}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11565" activeTab="5" xr2:uid="{9BE3A67C-EAA8-497E-B715-2E5EA49CD856}"/>
   </bookViews>
   <sheets>
-    <sheet name="1d" sheetId="2" r:id="rId1"/>
-    <sheet name="2d" sheetId="3" r:id="rId2"/>
-    <sheet name="missing_values" sheetId="1" r:id="rId3"/>
-    <sheet name="missing_axis_name" sheetId="6" r:id="rId4"/>
-    <sheet name="narrow_2d" sheetId="8" r:id="rId5"/>
+    <sheet name="pop" sheetId="1" r:id="rId1"/>
+    <sheet name="births" sheetId="2" r:id="rId2"/>
+    <sheet name="deaths" sheetId="3" r:id="rId3"/>
+    <sheet name="pop_missing_axis_name" sheetId="4" r:id="rId4"/>
+    <sheet name="pop_missing_values" sheetId="5" r:id="rId5"/>
+    <sheet name="pop_narrow_format" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="10">
   <si>
-    <t>a</t>
+    <t>geo</t>
   </si>
   <si>
-    <t>b\c</t>
+    <t>gender\time</t>
   </si>
   <si>
-    <t>c0</t>
+    <t>Belgium</t>
   </si>
   <si>
-    <t>c1</t>
+    <t>Male</t>
   </si>
   <si>
-    <t>c2</t>
+    <t>Female</t>
   </si>
   <si>
-    <t>a0</t>
+    <t>France</t>
   </si>
   <si>
-    <t>b0</t>
+    <t>Germany</t>
   </si>
   <si>
-    <t>b1</t>
+    <t>gender</t>
   </si>
   <si>
-    <t>b2</t>
-  </si>
-  <si>
-    <t>a1</t>
-  </si>
-  <si>
-    <t>a2</t>
-  </si>
-  <si>
-    <t>a\b</t>
-  </si>
-  <si>
-    <t>b</t>
+    <t>time</t>
   </si>
   <si>
     <t>value</t>
@@ -421,36 +415,130 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB771114-7E9D-4C17-8B40-9DF1002A104F}">
-  <dimension ref="A1:D2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9C4059-1A00-45BB-9BA1-67B1A2124563}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2013</v>
+      </c>
+      <c r="D1">
+        <v>2014</v>
+      </c>
+      <c r="E1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>5472856</v>
+      </c>
+      <c r="D2">
+        <v>5493792</v>
+      </c>
+      <c r="E2">
+        <v>5524068</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>5665118</v>
+      </c>
+      <c r="D3">
+        <v>5687048</v>
+      </c>
+      <c r="E3">
+        <v>5713206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>5</v>
       </c>
-      <c r="C1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>31772665</v>
+      </c>
+      <c r="D4">
+        <v>31936596</v>
+      </c>
+      <c r="E4">
+        <v>32175328</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>33827685</v>
+      </c>
+      <c r="D5">
+        <v>34005671</v>
+      </c>
+      <c r="E5">
+        <v>34280951</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>39380976</v>
+      </c>
+      <c r="D6">
+        <v>39556923</v>
+      </c>
+      <c r="E6">
+        <v>39835457</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>41142770</v>
+      </c>
+      <c r="D7">
+        <v>41210540</v>
+      </c>
+      <c r="E7">
+        <v>41362080</v>
       </c>
     </row>
   </sheetData>
@@ -459,57 +547,130 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C0E2D3-3AD2-443A-B350-378AA4CCC2E1}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF006A08-AC77-4386-BFE4-006449F111EF}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2013</v>
+      </c>
+      <c r="D1">
+        <v>2014</v>
+      </c>
+      <c r="E1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>64371</v>
+      </c>
+      <c r="D2">
+        <v>64173</v>
+      </c>
+      <c r="E2">
+        <v>62561</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>61235</v>
+      </c>
+      <c r="D3">
+        <v>60841</v>
+      </c>
+      <c r="E3">
+        <v>59713</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>415762</v>
+      </c>
+      <c r="D4">
+        <v>418721</v>
+      </c>
+      <c r="E4">
+        <v>409145</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>396581</v>
+      </c>
+      <c r="D5">
+        <v>400607</v>
+      </c>
+      <c r="E5">
+        <v>390526</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-      <c r="C4">
-        <v>5</v>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>349820</v>
+      </c>
+      <c r="D6">
+        <v>366835</v>
+      </c>
+      <c r="E6">
+        <v>378478</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>332249</v>
+      </c>
+      <c r="D7">
+        <v>348092</v>
+      </c>
+      <c r="E7">
+        <v>359097</v>
       </c>
     </row>
   </sheetData>
@@ -518,12 +679,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F29D973-230B-4F35-A565-0C438B724252}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B4A8AD-D7C2-4B7B-8B0F-F69E8F4403CD}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -534,82 +693,116 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+      <c r="C1">
+        <v>2013</v>
+      </c>
+      <c r="D1">
+        <v>2014</v>
+      </c>
+      <c r="E1">
+        <v>2015</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>2</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>53908</v>
+      </c>
+      <c r="D2">
+        <v>51579</v>
+      </c>
+      <c r="E2">
+        <v>53631</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>55426</v>
+      </c>
+      <c r="D3">
+        <v>53176</v>
+      </c>
+      <c r="E3">
+        <v>56910</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>287410</v>
+      </c>
+      <c r="D4">
+        <v>282381</v>
+      </c>
+      <c r="E4">
+        <v>297028</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>281955</v>
+      </c>
+      <c r="D5">
+        <v>277054</v>
+      </c>
+      <c r="E5">
+        <v>296779</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>4</v>
-      </c>
-      <c r="E3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4">
-        <v>9</v>
-      </c>
-      <c r="D4">
-        <v>10</v>
-      </c>
-      <c r="E4">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>429645</v>
+      </c>
+      <c r="D6">
+        <v>422225</v>
+      </c>
+      <c r="E6">
+        <v>449512</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="C5">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>13</v>
-      </c>
-      <c r="E5">
-        <v>14</v>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>464180</v>
+      </c>
+      <c r="D7">
+        <v>446131</v>
+      </c>
+      <c r="E7">
+        <v>475688</v>
       </c>
     </row>
   </sheetData>
@@ -618,69 +811,130 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D81E4C1A-F6DA-48F4-A82B-E5C5AF5C5575}">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BD980BD-847F-498C-9397-1BF4A1E12CBA}">
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1">
+        <v>2013</v>
+      </c>
+      <c r="D1">
+        <v>2014</v>
+      </c>
+      <c r="E1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>5472856</v>
+      </c>
+      <c r="D2">
+        <v>5493792</v>
+      </c>
+      <c r="E2">
+        <v>5524068</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>5665118</v>
+      </c>
+      <c r="D3">
+        <v>5687048</v>
+      </c>
+      <c r="E3">
+        <v>5713206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>31772665</v>
+      </c>
+      <c r="D4">
+        <v>31936596</v>
+      </c>
+      <c r="E4">
+        <v>32175328</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>33827685</v>
+      </c>
+      <c r="D5">
+        <v>34005671</v>
+      </c>
+      <c r="E5">
+        <v>34280951</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4">
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>39380976</v>
+      </c>
+      <c r="D6">
+        <v>39556923</v>
+      </c>
+      <c r="E6">
+        <v>39835457</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="C4">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>8</v>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>41142770</v>
+      </c>
+      <c r="D7">
+        <v>41210540</v>
+      </c>
+      <c r="E7">
+        <v>41362080</v>
       </c>
     </row>
   </sheetData>
@@ -689,12 +943,108 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38031E58-3461-4A03-B842-9AEABFC0F6E2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD6C4D3-5A4A-49C7-BA9C-7562042A28B2}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2013</v>
+      </c>
+      <c r="D1">
+        <v>2014</v>
+      </c>
+      <c r="E1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>5472856</v>
+      </c>
+      <c r="D2">
+        <v>5493792</v>
+      </c>
+      <c r="E2">
+        <v>5524068</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>5665118</v>
+      </c>
+      <c r="D3">
+        <v>5687048</v>
+      </c>
+      <c r="E3">
+        <v>5713206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>33827685</v>
+      </c>
+      <c r="D4">
+        <v>34005671</v>
+      </c>
+      <c r="E4">
+        <v>34280951</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>39380976</v>
+      </c>
+      <c r="D5">
+        <v>39556923</v>
+      </c>
+      <c r="E5">
+        <v>39835457</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5258A7-89D3-4939-9C47-DA8F443C2E19}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -703,80 +1053,79 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>2013</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>11137974</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2014</v>
       </c>
       <c r="C3">
-        <v>1</v>
+        <v>11180840</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>2015</v>
       </c>
       <c r="C4">
-        <v>2</v>
+        <v>11237274</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>2013</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>65600350</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>3</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2014</v>
       </c>
       <c r="C6">
-        <v>4</v>
+        <v>65942267</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
-        <v>7</v>
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2015</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>66456279</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="599" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added range argument to read_excel
</commit_message>
<xml_diff>
--- a/larray/tests/data/examples.xlsx
+++ b/larray/tests/data/examples.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ald\Projects\larray\larray\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083B36A3-412C-4F86-872C-2976BE7F79A2}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DEA03F1-CFA6-43AA-84C9-A28FB00E85DD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11565" activeTab="5" xr2:uid="{9BE3A67C-EAA8-497E-B715-2E5EA49CD856}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="11565" firstSheet="2" activeTab="6" xr2:uid="{A12C254C-960A-4AAF-85FF-7581D4D82B16}"/>
   </bookViews>
   <sheets>
     <sheet name="pop" sheetId="1" r:id="rId1"/>
     <sheet name="births" sheetId="2" r:id="rId2"/>
     <sheet name="deaths" sheetId="3" r:id="rId3"/>
-    <sheet name="pop_missing_axis_name" sheetId="4" r:id="rId4"/>
-    <sheet name="pop_missing_values" sheetId="5" r:id="rId5"/>
-    <sheet name="pop_narrow_format" sheetId="6" r:id="rId6"/>
+    <sheet name="pop_births_deaths" sheetId="4" r:id="rId4"/>
+    <sheet name="pop_missing_axis_name" sheetId="5" r:id="rId5"/>
+    <sheet name="pop_missing_values" sheetId="6" r:id="rId6"/>
+    <sheet name="pop_narrow_format" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="179017"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="10">
   <si>
     <t>geo</t>
   </si>
@@ -415,7 +416,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F9C4059-1A00-45BB-9BA1-67B1A2124563}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61BE790E-79A9-470F-AB9B-29365D010FFB}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -547,7 +548,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF006A08-AC77-4386-BFE4-006449F111EF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0327710A-D949-4841-B2D2-5D1CA67153B6}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -679,7 +680,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40B4A8AD-D7C2-4B7B-8B0F-F69E8F4403CD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4116F0A1-81D1-4F38-B3D4-C942CFF6A2A3}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -811,7 +812,377 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BD980BD-847F-498C-9397-1BF4A1E12CBA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA00C9EF-42E5-4CB7-8653-AC9E9DA67E51}">
+  <dimension ref="A1:E23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2013</v>
+      </c>
+      <c r="D1">
+        <v>2014</v>
+      </c>
+      <c r="E1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>5472856</v>
+      </c>
+      <c r="D2">
+        <v>5493792</v>
+      </c>
+      <c r="E2">
+        <v>5524068</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>5665118</v>
+      </c>
+      <c r="D3">
+        <v>5687048</v>
+      </c>
+      <c r="E3">
+        <v>5713206</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>31772665</v>
+      </c>
+      <c r="D4">
+        <v>31936596</v>
+      </c>
+      <c r="E4">
+        <v>32175328</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <v>33827685</v>
+      </c>
+      <c r="D5">
+        <v>34005671</v>
+      </c>
+      <c r="E5">
+        <v>34280951</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6">
+        <v>39380976</v>
+      </c>
+      <c r="D6">
+        <v>39556923</v>
+      </c>
+      <c r="E6">
+        <v>39835457</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>41142770</v>
+      </c>
+      <c r="D7">
+        <v>41210540</v>
+      </c>
+      <c r="E7">
+        <v>41362080</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>2013</v>
+      </c>
+      <c r="D9">
+        <v>2014</v>
+      </c>
+      <c r="E9">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10">
+        <v>64371</v>
+      </c>
+      <c r="D10">
+        <v>64173</v>
+      </c>
+      <c r="E10">
+        <v>62561</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>61235</v>
+      </c>
+      <c r="D11">
+        <v>60841</v>
+      </c>
+      <c r="E11">
+        <v>59713</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12">
+        <v>415762</v>
+      </c>
+      <c r="D12">
+        <v>418721</v>
+      </c>
+      <c r="E12">
+        <v>409145</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13">
+        <v>396581</v>
+      </c>
+      <c r="D13">
+        <v>400607</v>
+      </c>
+      <c r="E13">
+        <v>390526</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>349820</v>
+      </c>
+      <c r="D14">
+        <v>366835</v>
+      </c>
+      <c r="E14">
+        <v>378478</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>332249</v>
+      </c>
+      <c r="D15">
+        <v>348092</v>
+      </c>
+      <c r="E15">
+        <v>359097</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17">
+        <v>2013</v>
+      </c>
+      <c r="D17">
+        <v>2014</v>
+      </c>
+      <c r="E17">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>2</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>53908</v>
+      </c>
+      <c r="D18">
+        <v>51579</v>
+      </c>
+      <c r="E18">
+        <v>53631</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>55426</v>
+      </c>
+      <c r="D19">
+        <v>53176</v>
+      </c>
+      <c r="E19">
+        <v>56910</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20">
+        <v>287410</v>
+      </c>
+      <c r="D20">
+        <v>282381</v>
+      </c>
+      <c r="E20">
+        <v>297028</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4</v>
+      </c>
+      <c r="C21">
+        <v>281955</v>
+      </c>
+      <c r="D21">
+        <v>277054</v>
+      </c>
+      <c r="E21">
+        <v>296779</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3</v>
+      </c>
+      <c r="C22">
+        <v>429645</v>
+      </c>
+      <c r="D22">
+        <v>422225</v>
+      </c>
+      <c r="E22">
+        <v>449512</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>6</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23">
+        <v>464180</v>
+      </c>
+      <c r="D23">
+        <v>446131</v>
+      </c>
+      <c r="E23">
+        <v>475688</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23D4308D-6458-4352-9E6C-1C6F36A9FBA8}">
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -942,8 +1313,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD6C4D3-5A4A-49C7-BA9C-7562042A28B2}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2C4D986-8E59-4841-B8FE-54AC67906118}">
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1040,8 +1411,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5258A7-89D3-4939-9C47-DA8F443C2E19}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E962BC3-C541-4963-B396-0F3DF2576321}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>